<commit_message>
Updated harmonic, katz and subgraph results
</commit_message>
<xml_diff>
--- a/results/aucs/harmonic_centrality/aucs_harmonic_centrality_results.xlsx
+++ b/results/aucs/harmonic_centrality/aucs_harmonic_centrality_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>coauthor</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>shannon_entropy</t>
+  </si>
+  <si>
+    <t>cluster_class</t>
   </si>
   <si>
     <t>U1</t>
@@ -604,13 +607,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,10 +632,13 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1.32</v>
@@ -652,10 +658,13 @@
       <c r="G2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1.33</v>
@@ -675,10 +684,13 @@
       <c r="G3">
         <v>2.04</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -698,10 +710,13 @@
       <c r="G4">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>1.46</v>
@@ -721,10 +736,13 @@
       <c r="G5">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>0.82</v>
@@ -744,10 +762,13 @@
       <c r="G6">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>0.75</v>
@@ -767,10 +788,13 @@
       <c r="G7">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>4.58</v>
@@ -790,10 +814,13 @@
       <c r="G8">
         <v>2.11</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>0.6899999999999999</v>
@@ -813,10 +840,13 @@
       <c r="G9">
         <v>1.76</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>0.93</v>
@@ -836,10 +866,13 @@
       <c r="G10">
         <v>2.03</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>1.51</v>
@@ -859,10 +892,13 @@
       <c r="G11">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0.64</v>
@@ -882,10 +918,13 @@
       <c r="G12">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>0.88</v>
@@ -905,10 +944,13 @@
       <c r="G13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0.36</v>
@@ -928,10 +970,13 @@
       <c r="G14">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>1.54</v>
@@ -951,10 +996,13 @@
       <c r="G15">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>4.24</v>
@@ -974,10 +1022,13 @@
       <c r="G16">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>2.54</v>
@@ -997,10 +1048,13 @@
       <c r="G17">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>3.26</v>
@@ -1020,10 +1074,13 @@
       <c r="G18">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1043,10 +1100,13 @@
       <c r="G19">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>0.52</v>
@@ -1066,10 +1126,13 @@
       <c r="G20">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1089,10 +1152,13 @@
       <c r="G21">
         <v>0.28</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>0.35</v>
@@ -1112,10 +1178,13 @@
       <c r="G22">
         <v>1.71</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>1.46</v>
@@ -1135,10 +1204,13 @@
       <c r="G23">
         <v>2.05</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>0.49</v>
@@ -1158,10 +1230,13 @@
       <c r="G24">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>3.41</v>
@@ -1181,10 +1256,13 @@
       <c r="G25">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>0.39</v>
@@ -1204,10 +1282,13 @@
       <c r="G26">
         <v>1.68</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>0.79</v>
@@ -1227,10 +1308,13 @@
       <c r="G27">
         <v>1.98</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>1.51</v>
@@ -1250,10 +1334,13 @@
       <c r="G28">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>0.52</v>
@@ -1273,10 +1360,13 @@
       <c r="G29">
         <v>1.83</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>1.14</v>
@@ -1296,10 +1386,13 @@
       <c r="G30">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>1.45</v>
@@ -1319,10 +1412,13 @@
       <c r="G31">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>0.72</v>
@@ -1342,10 +1438,13 @@
       <c r="G32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>1.44</v>
@@ -1365,10 +1464,13 @@
       <c r="G33">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -1388,10 +1490,13 @@
       <c r="G34">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>0.33</v>
@@ -1411,10 +1516,13 @@
       <c r="G35">
         <v>1.76</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>0.77</v>
@@ -1434,10 +1542,13 @@
       <c r="G36">
         <v>1.87</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>1.55</v>
@@ -1457,10 +1568,13 @@
       <c r="G37">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1480,10 +1594,13 @@
       <c r="G38">
         <v>2.01</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <v>3.41</v>
@@ -1503,10 +1620,13 @@
       <c r="G39">
         <v>2.08</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B40">
         <v>1.37</v>
@@ -1526,10 +1646,13 @@
       <c r="G40">
         <v>1.54</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41">
         <v>0.87</v>
@@ -1549,10 +1672,13 @@
       <c r="G41">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42">
         <v>5.3</v>
@@ -1572,10 +1698,13 @@
       <c r="G42">
         <v>2.08</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43">
         <v>0.7</v>
@@ -1595,10 +1724,13 @@
       <c r="G43">
         <v>2.01</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44">
         <v>0.96</v>
@@ -1618,10 +1750,13 @@
       <c r="G44">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45">
         <v>0.72</v>
@@ -1641,10 +1776,13 @@
       <c r="G45">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46">
         <v>0.33</v>
@@ -1664,10 +1802,13 @@
       <c r="G46">
         <v>1.64</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1687,10 +1828,13 @@
       <c r="G47">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B48">
         <v>0.86</v>
@@ -1710,10 +1854,13 @@
       <c r="G48">
         <v>2.05</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49">
         <v>0.79</v>
@@ -1733,10 +1880,13 @@
       <c r="G49">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>1.42</v>
@@ -1756,10 +1906,13 @@
       <c r="G50">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51">
         <v>0.74</v>
@@ -1779,10 +1932,13 @@
       <c r="G51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B52">
         <v>0.74</v>
@@ -1802,10 +1958,13 @@
       <c r="G52">
         <v>1.67</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>3.13</v>
@@ -1825,10 +1984,13 @@
       <c r="G53">
         <v>1.94</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>0.5600000000000001</v>
@@ -1848,10 +2010,13 @@
       <c r="G54">
         <v>1.86</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>3.1</v>
@@ -1871,10 +2036,13 @@
       <c r="G55">
         <v>2.11</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>0.79</v>
@@ -1894,10 +2062,13 @@
       <c r="G56">
         <v>2.02</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B57">
         <v>0.74</v>
@@ -1917,10 +2088,13 @@
       <c r="G57">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B58">
         <v>0.36</v>
@@ -1940,10 +2114,13 @@
       <c r="G58">
         <v>1.74</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59">
         <v>2.75</v>
@@ -1963,10 +2140,13 @@
       <c r="G59">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B60">
         <v>0.02</v>
@@ -1986,10 +2166,13 @@
       <c r="G60">
         <v>1.33</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B61">
         <v>3.84</v>
@@ -2009,10 +2192,13 @@
       <c r="G61">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B62">
         <v>3.97</v>
@@ -2032,10 +2218,13 @@
       <c r="G62">
         <v>1.92</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B63">
         <v>1.35</v>
@@ -2054,6 +2243,9 @@
       </c>
       <c r="G63">
         <v>1.79</v>
+      </c>
+      <c r="H63">
+        <v>-0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>